<commit_message>
feat. ata e sprint backlog sprint 3
</commit_message>
<xml_diff>
--- a/SprintBackLog.xlsx
+++ b/SprintBackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PI\API-Acolhe-SP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C101563-00D9-4E71-A44F-55FC1F8BD9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EED5193-3EAA-4DC9-BFB9-4B15B6064AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{18D2300B-313B-43F3-B969-E9BE2C22E98B}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Acolhe-SP</t>
   </si>
@@ -81,14 +80,75 @@
   </si>
   <si>
     <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Integrar Front-end com Back-end</t>
+  </si>
+  <si>
+    <t>Itallo/Gabriel</t>
+  </si>
+  <si>
+    <t>Não começou</t>
+  </si>
+  <si>
+    <t>Integrar nosso sistema com API GerenciaNET</t>
+  </si>
+  <si>
+    <t>Gabriel - sub(Itallo)</t>
+  </si>
+  <si>
+    <t>Itallo - sub(Gabriel)</t>
+  </si>
+  <si>
+    <t>Integrar com API de GeoLocalização</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Integrar com API CEP-promisse</t>
+  </si>
+  <si>
+    <t>Documentação do projeto atualizada</t>
+  </si>
+  <si>
+    <t>PPT de apresentação do projeto</t>
+  </si>
+  <si>
+    <t>White Papper do projeto</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Relatório</t>
+  </si>
+  <si>
+    <t>Testes Junit</t>
+  </si>
+  <si>
+    <t>Front Dashboard</t>
+  </si>
+  <si>
+    <t>Integrar os dados do back-end com o front-end</t>
+  </si>
+  <si>
+    <t>Itallo</t>
+  </si>
+  <si>
+    <t>Victória</t>
+  </si>
+  <si>
+    <t>Raoan/Luan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-416]d\-mmm;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -129,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +214,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -275,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,39 +360,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -336,53 +406,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,15 +788,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B577208-F413-413D-97B0-1FD462443434}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
@@ -718,74 +806,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="11"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="33"/>
+      <c r="P1" s="39"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="34"/>
+      <c r="P2" s="35"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="35"/>
+      <c r="P3" s="40"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="6"/>
@@ -796,6 +884,10 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
+      <c r="O4" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="38"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -804,301 +896,410 @@
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="1:19" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="20" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="20" t="s">
+      <c r="I8" s="23"/>
+      <c r="J8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="K8" s="22"/>
+    </row>
+    <row r="9" spans="1:19" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-    </row>
-    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="B9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="43">
+        <v>44696</v>
+      </c>
+      <c r="I9" s="43"/>
+      <c r="J9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="35"/>
+    </row>
+    <row r="10" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="B10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="43">
+        <v>44696</v>
+      </c>
+      <c r="I10" s="43"/>
+      <c r="J10" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>3</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="B11" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="36"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="43">
+        <v>44696</v>
+      </c>
+      <c r="I11" s="43"/>
+      <c r="J11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="38"/>
+    </row>
+    <row r="12" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="B12" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="43">
+        <v>44688</v>
+      </c>
+      <c r="I12" s="43"/>
+      <c r="J12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="38"/>
+    </row>
+    <row r="13" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>5</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="B13" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="44">
+        <v>44688</v>
+      </c>
+      <c r="I13" s="44"/>
+      <c r="J13" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="38"/>
+    </row>
+    <row r="14" spans="1:19" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>6</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="B14" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="44">
+        <v>44690</v>
+      </c>
+      <c r="I14" s="44"/>
+      <c r="J14" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="38"/>
+    </row>
+    <row r="15" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>7</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="B15" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="44">
+        <v>44701</v>
+      </c>
+      <c r="I15" s="44"/>
+      <c r="J15" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="35"/>
+    </row>
+    <row r="16" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>8</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="B16" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="44">
+        <v>44701</v>
+      </c>
+      <c r="I16" s="44"/>
+      <c r="J16" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="38"/>
+    </row>
+    <row r="17" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>9</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="B17" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="36"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="44">
+        <v>44701</v>
+      </c>
+      <c r="I17" s="44"/>
+      <c r="J17" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="38"/>
+    </row>
+    <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <v>10</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="B18" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="44">
+        <v>44696</v>
+      </c>
+      <c r="I18" s="44"/>
+      <c r="J18" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="38"/>
+    </row>
+    <row r="19" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>11</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="44">
+        <v>44701</v>
+      </c>
+      <c r="I19" s="44"/>
+      <c r="J19" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="38"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="68">
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="O3:P3"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
     <mergeCell ref="D1:K3"/>
     <mergeCell ref="B5:K5"/>
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>